<commit_message>
Added v6 RPM tags + logging duplicates + keeping headers in properties
</commit_message>
<xml_diff>
--- a/Rpm Tags.xlsx
+++ b/Rpm Tags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pascal\Documents\Developpement\git.arx.one\get.arx.one\RpmReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B31982-B07C-429C-B3AF-C5DE074E92B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F562706-F91B-4318-AF21-085382651398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F0417157-B67F-4D97-A111-30F8D637A2CB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="422">
   <si>
     <t>Name</t>
   </si>
@@ -1998,10 +1998,46 @@
     <t>Enum</t>
   </si>
   <si>
-    <t>Fileclass2</t>
-  </si>
-  <si>
     <t>https://rpm-software-management.github.io/rpm/manual/tags.html</t>
+  </si>
+  <si>
+    <t>HEADERSIGNATURES</t>
+  </si>
+  <si>
+    <t>BIN</t>
+  </si>
+  <si>
+    <t>DSA</t>
+  </si>
+  <si>
+    <t>RSA</t>
+  </si>
+  <si>
+    <t>SHA256</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>FILESIGNATURES</t>
+  </si>
+  <si>
+    <t>STRING_ARRAY</t>
+  </si>
+  <si>
+    <t>VERITYSIGNATURES</t>
+  </si>
+  <si>
+    <t>VERITYSIGNATUREALGO</t>
+  </si>
+  <si>
+    <t>INT_32</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
+  </si>
+  <si>
+    <t>FileClass</t>
   </si>
 </sst>
 </file>
@@ -2058,7 +2094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2084,6 +2120,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2123,15 +2162,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F9EEF87-1B9F-4364-ADE3-1F3154F473A4}" name="Tableau1" displayName="Tableau1" ref="A2:E264" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A2:E264" xr:uid="{1F9EEF87-1B9F-4364-ADE3-1F3154F473A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F9EEF87-1B9F-4364-ADE3-1F3154F473A4}" name="Tableau1" displayName="Tableau1" ref="A2:E273" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A2:E273" xr:uid="{1F9EEF87-1B9F-4364-ADE3-1F3154F473A4}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BD886ED9-34DB-4F8E-BE84-096008961462}" name="Tag" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B7875AD0-9A65-4F57-8096-482104826987}" name="Value" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{3AB8B8EA-4529-415B-8985-1602511EB0E6}" name="Type" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{BD5594FD-4038-406A-B9F7-A4255C186C62}" name="Description" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{53167BB1-172C-4E80-B94E-2E7F48FF884F}" name="Enum" dataDxfId="0">
-      <calculatedColumnFormula>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2455,9 +2494,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84458CB8-CBB3-4032-B380-82A0424FE9FA}">
-  <dimension ref="A1:E264"/>
+  <dimension ref="A1:E273"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="A246" sqref="A246"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -2469,7 +2510,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2497,7 +2538,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// === Base package tags</v>
       </c>
     </row>
@@ -2515,8 +2556,8 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Name = 1000, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Name = 1000, // (string) Package name.</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2533,8 +2574,8 @@
         <v>4</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Version = 1001, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Version = 1001, // (string) Package version.</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2551,8 +2592,8 @@
         <v>6</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Release = 1002, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Release = 1002, // (string) Package release.</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2569,8 +2610,8 @@
         <v>9</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Epoch = 1003, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Epoch = 1003, // (int32) Package epoch (optional). An absent epoch is equal to epoch value 0.</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2587,8 +2628,8 @@
         <v>11</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>License = 1014, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>License = 1014, // (string) License of the package contents.</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2605,8 +2646,8 @@
         <v>14</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Summary = 1004, // i18nstring</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Summary = 1004, // (i18nstring) One line summary of the package’s purpose.</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2623,8 +2664,8 @@
         <v>16</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Description = 1005, // i18nstring</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Description = 1005, // (i18nstring) Multiline description of the package’s purpose</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2641,8 +2682,8 @@
         <v>18</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Os = 1021, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Os = 1021, // (string) The operating system the package is for</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2659,8 +2700,8 @@
         <v>20</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Arch = 1022, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Arch = 1022, // (string) The architecture the package is for. noarch is a special case denoting a architecture independent package.</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="24">
@@ -2671,7 +2712,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// === Informative package tags</v>
       </c>
     </row>
@@ -2689,8 +2730,8 @@
         <v>27</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Buildhost = 1007, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Buildhost = 1007, // (string) Hostname of the system the package was built on.</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2707,8 +2748,8 @@
         <v>29</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Buildtime = 1006, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Buildtime = 1006, // (int32) Unix timestamp of package build time.</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2725,8 +2766,8 @@
         <v>31</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Bugurl = 5012, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Bugurl = 5012, // (string) URL to package bug tracker.</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2743,8 +2784,8 @@
         <v>34</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Changelogname = 1081, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Changelogname = 1081, // (string array) Per entry changelog author information, typically name &lt;email&gt;.</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2761,8 +2802,8 @@
         <v>36</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Changelogtext = 1082, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Changelogtext = 1082, // (string array) Per entry changelog text.</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2779,8 +2820,8 @@
         <v>39</v>
       </c>
       <c r="E19" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Changelogtime = 1080, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Changelogtime = 1080, // (int32 array) Per entry changelog Unix timestamp.</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2797,8 +2838,8 @@
         <v>41</v>
       </c>
       <c r="E20" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Cookie = 1094, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Cookie = 1094, // (string) An opaque value for tracking packages from a single build operation.</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2815,8 +2856,8 @@
         <v>43</v>
       </c>
       <c r="E21" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Distribution = 1010, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Distribution = 1010, // (string) Distribution name.</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2833,8 +2874,8 @@
         <v>45</v>
       </c>
       <c r="E22" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Disttag = 1155, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Disttag = 1155, // (string) Distribution acronym.</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2851,8 +2892,8 @@
         <v>47</v>
       </c>
       <c r="E23" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Disturl = 1123, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Disturl = 1123, // (string) Distribution specific URL of the package.</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2869,8 +2910,8 @@
         <v>49</v>
       </c>
       <c r="E24" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Encoding = 5062, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Encoding = 5062, // (string) Encoding of the header string data. When present it is always utf-8 and the data has actually been validated.</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2887,8 +2928,8 @@
         <v>51</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Group = 1016, // i18nstring</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Group = 1016, // (i18nstring) Group of the package.</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2903,8 +2944,8 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Modularitylabel = 5096, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Modularitylabel = 5096, // (string) </v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2921,8 +2962,8 @@
         <v>54</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Optflags = 1122, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Optflags = 1122, // (string) %{optflags} value at the time of package build.</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2939,8 +2980,8 @@
         <v>56</v>
       </c>
       <c r="E28" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Packager = 1015, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Packager = 1015, // (string) Packager contact information.</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2957,8 +2998,8 @@
         <v>58</v>
       </c>
       <c r="E29" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Platform = 1132, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Platform = 1132, // (string) Package platform (arch-os-vendor).</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2973,8 +3014,8 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Policies = 1150, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Policies = 1150, // (string array) </v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2989,8 +3030,8 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Policyflags = 5033, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Policyflags = 5033, // (int32 array) </v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3005,8 +3046,8 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Policynames = 5030, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Policynames = 5030, // (string array) </v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3021,8 +3062,8 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Policytypes = 5031, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Policytypes = 5031, // (string array) </v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3037,8 +3078,8 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Policytypesindexes = 5032, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Policytypesindexes = 5032, // (int32 array) </v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3055,8 +3096,8 @@
         <v>65</v>
       </c>
       <c r="E35" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Rpmversion = 1064, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Rpmversion = 1064, // (string) Version of rpm used to build the package.</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3071,8 +3112,8 @@
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sourcepkgid = 1146, // bin</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Sourcepkgid = 1146, // (bin) </v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3089,8 +3130,8 @@
         <v>69</v>
       </c>
       <c r="E37" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sourcerpm = 1044, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sourcerpm = 1044, // (string) Package source rpm file name.</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3107,8 +3148,8 @@
         <v>71</v>
       </c>
       <c r="E38" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Translationurl = 5100, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Translationurl = 5100, // (string) URL of upstream translation service/repository</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30">
@@ -3125,8 +3166,8 @@
         <v>73</v>
       </c>
       <c r="E39" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>UpstreamReleases = 5101, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>UpstreamReleases = 5101, // (string) URL to check for newer releases from upstream e.g. for build systems to check for newer upstream releases and then to notify the packager.</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3143,8 +3184,8 @@
         <v>75</v>
       </c>
       <c r="E40" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Url = 1020, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Url = 1020, // (string) Package URL, typically project upstream website.</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="45">
@@ -3161,8 +3202,8 @@
         <v>77</v>
       </c>
       <c r="E41" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Vcs = 5034, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Vcs = 5034, // (string) (Public) upstream source code VCS location. Format &lt;vcs&gt;:&lt;address&gt; with &lt;vcs&gt; being the VCS command used (e.g. git, svn, hg, …) and &lt;address&gt; being the location of the repository as used by the VCS tool to clone/checkout the repository (e.g. https://github.com/rpm-software-management/rpm.git).</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3179,8 +3220,8 @@
         <v>79</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Vendor = 1011, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Vendor = 1011, // (string) Package vendor contact information.</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="24">
@@ -3191,7 +3232,7 @@
         <v>80</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// === Packages with files</v>
       </c>
     </row>
@@ -3209,8 +3250,8 @@
         <v>82</v>
       </c>
       <c r="E44" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Archivesize = 1046, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Archivesize = 1046, // (int32) (Uncompressed) payload size.</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3227,8 +3268,8 @@
         <v>84</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Dirnames = 1118, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Dirnames = 1118, // (string array) dirname(3) components of contained paths</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3245,8 +3286,8 @@
         <v>86</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filedigestalgo = 5011, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filedigestalgo = 5011, // (int32) ID of file digest algorithm. If missing, considered 0 for md5.</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3263,8 +3304,8 @@
         <v>89</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Longarchivesize = 271, // int64</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Longarchivesize = 271, // (int64) (Uncompressed) payload size when &gt; 4GB.</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -3281,8 +3322,8 @@
         <v>91</v>
       </c>
       <c r="E48" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Longsize = 5009, // int64</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Longsize = 5009, // (int64) Installed package size when &gt; 4GB.</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3299,8 +3340,8 @@
         <v>93</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Payloadcompressor = 1125, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Payloadcompressor = 1125, // (string) Payload compressor name (as passed to rpmio Fopen())</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3317,8 +3358,8 @@
         <v>95</v>
       </c>
       <c r="E50" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Payloadflags = 1126, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Payloadflags = 1126, // (string) Payload compressor level (as passed to rpmio Fopen())</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3335,8 +3376,8 @@
         <v>97</v>
       </c>
       <c r="E51" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Payloadformat = 1124, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Payloadformat = 1124, // (string) Payload format (cpio)</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3353,8 +3394,8 @@
         <v>99</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Prefixes = 1098, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Prefixes = 1098, // (string array) Relocatable prefixes (on relocatable packages).</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3371,8 +3412,8 @@
         <v>101</v>
       </c>
       <c r="E53" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Size = 1009, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Size = 1009, // (int32) Installed package size.</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="24">
@@ -3383,7 +3424,7 @@
         <v>102</v>
       </c>
       <c r="E54" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// === Per-file information</v>
       </c>
     </row>
@@ -3401,8 +3442,8 @@
         <v>104</v>
       </c>
       <c r="E55" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Basenames = 1117, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Basenames = 1117, // (string array) basename(3) of the path.</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3419,8 +3460,8 @@
         <v>106</v>
       </c>
       <c r="E56" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Dirindexes = 1116, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Dirindexes = 1116, // (int32 array) Index into dirname(3) array of the pacakge (see Dirname tag).</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3437,8 +3478,8 @@
         <v>108</v>
       </c>
       <c r="E57" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filedevices = 1095, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filedevices = 1095, // (int32 array) Abstract device ID (hardlink calculation only).</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3455,8 +3496,8 @@
         <v>110</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filedigests = 1035, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filedigests = 1035, // (string array) File cryptographic digest (aka hash) using algorithm specified in Filedigestalgo.</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3473,8 +3514,8 @@
         <v>112</v>
       </c>
       <c r="E59" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fileflags = 1037, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Fileflags = 1037, // (int32 array) File virtual attributes (doc, license, ghost, artifact etc)</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3491,8 +3532,8 @@
         <v>114</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filegroupname = 1040, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filegroupname = 1040, // (string array) Unix group name.</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3509,8 +3550,8 @@
         <v>116</v>
       </c>
       <c r="E61" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fileinodes = 1096, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Fileinodes = 1096, // (int32 array) Abstract inode number (hardlink calculation only).</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3527,8 +3568,8 @@
         <v>118</v>
       </c>
       <c r="E62" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filelangs = 1097, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filelangs = 1097, // (string array) Optional language of the file (eg man page translations)</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3545,8 +3586,8 @@
         <v>120</v>
       </c>
       <c r="E63" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filelinktos = 1036, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filelinktos = 1036, // (string array) Symlink target for symlink files.</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3563,8 +3604,8 @@
         <v>123</v>
       </c>
       <c r="E64" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filemodes = 1030, // int16 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filemodes = 1030, // (int16 array) Unix file mode.</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3581,8 +3622,8 @@
         <v>125</v>
       </c>
       <c r="E65" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filemtimes = 1034, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filemtimes = 1034, // (int32 array) Unix file modification timestamp (aka mtime).</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3599,8 +3640,8 @@
         <v>127</v>
       </c>
       <c r="E66" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filerdevs = 1033, // int16 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filerdevs = 1033, // (int16 array) Device ID (of device files)</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3617,8 +3658,8 @@
         <v>129</v>
       </c>
       <c r="E67" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filesizes = 1028, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filesizes = 1028, // (int32 array) File size (when all files are &lt; 4GB)</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3635,8 +3676,8 @@
         <v>131</v>
       </c>
       <c r="E68" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fileusername = 1039, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Fileusername = 1039, // (string array) Unix owner name</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3653,8 +3694,8 @@
         <v>133</v>
       </c>
       <c r="E69" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fileverifyflags = 1045, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Fileverifyflags = 1045, // (int32 array) File verification flags (which aspects of file to verify)</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3671,8 +3712,8 @@
         <v>136</v>
       </c>
       <c r="E70" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Longfilesizes = 5008, // int64 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Longfilesizes = 5008, // (int64 array) File size (when files &gt; 4GB are present)</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18">
@@ -3683,7 +3724,7 @@
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// --- Optional file information</v>
       </c>
     </row>
@@ -3701,8 +3742,8 @@
         <v>139</v>
       </c>
       <c r="E72" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Classdict = 1142, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Classdict = 1142, // (string array) File class (libmagic string) dictionary</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3719,8 +3760,8 @@
         <v>141</v>
       </c>
       <c r="E73" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Dependsdict = 1145, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Dependsdict = 1145, // (int32 array) File dependencies dictionary</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3737,8 +3778,8 @@
         <v>143</v>
       </c>
       <c r="E74" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filecaps = 5010, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filecaps = 5010, // (string array) cap_to_text(3) textual representation of file capabilities.</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3755,8 +3796,8 @@
         <v>145</v>
       </c>
       <c r="E75" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fileclass = 1141, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Fileclass = 1141, // (int32 array) Index into Classdict</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3773,8 +3814,8 @@
         <v>147</v>
       </c>
       <c r="E76" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filecolors = 1140, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filecolors = 1140, // (int32 array) File “color” - 1 for 32bit ELF, 2 for 64bit ELF and 0 otherwise</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3791,8 +3832,8 @@
         <v>149</v>
       </c>
       <c r="E77" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filedependsn = 1144, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filedependsn = 1144, // (int32 array) Number of file dependencies in Dependsdict, starting from Filedependsx</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -3809,8 +3850,8 @@
         <v>151</v>
       </c>
       <c r="E78" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filedependsx = 1143, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filedependsx = 1143, // (int32 array) Index into Dependsdict denoting start of this file’s dependencies.</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -3827,8 +3868,8 @@
         <v>153</v>
       </c>
       <c r="E79" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filesignaturelength = 5091, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filesignaturelength = 5091, // (int32) IMA signature length.</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -3845,8 +3886,8 @@
         <v>155</v>
       </c>
       <c r="E80" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filesignatures = 5090, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filesignatures = 5090, // (string array) IMA signature (hex encoded).</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3863,8 +3904,8 @@
         <v>157</v>
       </c>
       <c r="E81" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Veritysignaturealgo = 277, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Veritysignaturealgo = 277, // (int32) fsverity signature algorithm ID.</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3881,8 +3922,8 @@
         <v>159</v>
       </c>
       <c r="E82" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Veritysignatures = 276, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Veritysignatures = 276, // (string array) fsverity signature (base64 encoded).</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="24">
@@ -3893,7 +3934,7 @@
         <v>160</v>
       </c>
       <c r="E83" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// === Dependency information</v>
       </c>
     </row>
@@ -3905,7 +3946,7 @@
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// --- Hard dependencies</v>
       </c>
     </row>
@@ -3921,8 +3962,8 @@
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Providename = 1047, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Providename = 1047, // (string array) </v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -3937,8 +3978,8 @@
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Provideversion = 1113, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Provideversion = 1113, // (string array) </v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -3953,8 +3994,8 @@
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Provideflags = 1112, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Provideflags = 1112, // (int32 array) </v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3969,8 +4010,8 @@
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Requirename = 1049, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Requirename = 1049, // (string array) </v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -3985,8 +4026,8 @@
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Requireversion = 1050, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Requireversion = 1050, // (string array) </v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -4001,8 +4042,8 @@
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Requireflags = 1048, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Requireflags = 1048, // (int32 array) </v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4017,8 +4058,8 @@
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Conflictname = 1054, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Conflictname = 1054, // (string array) </v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4033,8 +4074,8 @@
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Conflictversion = 1055, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Conflictversion = 1055, // (string array) </v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4049,8 +4090,8 @@
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Conflictflags = 1053, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Conflictflags = 1053, // (int32 array) </v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -4065,8 +4106,8 @@
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Obsoletename = 1090, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Obsoletename = 1090, // (string array) </v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4081,8 +4122,8 @@
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Obsoleteversion = 1115, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Obsoleteversion = 1115, // (string array) </v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4097,8 +4138,8 @@
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Obsoleteflags = 1114, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Obsoleteflags = 1114, // (int32 array) </v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="18">
@@ -4109,7 +4150,7 @@
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// --- Soft dependencies</v>
       </c>
     </row>
@@ -4125,8 +4166,8 @@
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Enhancename = 5055, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Enhancename = 5055, // (string array) </v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4141,8 +4182,8 @@
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Enhanceversion = 5056, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Enhanceversion = 5056, // (string array) </v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4157,8 +4198,8 @@
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Enhanceflags = 5057, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Enhanceflags = 5057, // (int32 array) </v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4173,8 +4214,8 @@
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Recommendname = 5046, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Recommendname = 5046, // (string array) </v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4189,8 +4230,8 @@
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Recommendversion = 5047, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Recommendversion = 5047, // (string array) </v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4205,8 +4246,8 @@
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Recommendflags = 5048, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Recommendflags = 5048, // (int32 array) </v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -4221,8 +4262,8 @@
       </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Suggestname = 5049, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Suggestname = 5049, // (string array) </v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -4237,8 +4278,8 @@
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Suggestversion = 5050, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Suggestversion = 5050, // (string array) </v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4253,8 +4294,8 @@
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Suggestflags = 5051, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Suggestflags = 5051, // (int32 array) </v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4269,8 +4310,8 @@
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Supplementname = 5052, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Supplementname = 5052, // (string array) </v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -4285,8 +4326,8 @@
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Supplementversion = 5053, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Supplementversion = 5053, // (string array) </v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4301,8 +4342,8 @@
       </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Supplementflags = 5054, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Supplementflags = 5054, // (int32 array) </v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4317,8 +4358,8 @@
       </c>
       <c r="D110" s="1"/>
       <c r="E110" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Ordername = 5035, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Ordername = 5035, // (string array) </v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4333,8 +4374,8 @@
       </c>
       <c r="D111" s="1"/>
       <c r="E111" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Orderversion = 5036, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Orderversion = 5036, // (string array) </v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4349,8 +4390,8 @@
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Orderflags = 5037, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Orderflags = 5037, // (int32 array) </v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="24">
@@ -4361,7 +4402,7 @@
         <v>190</v>
       </c>
       <c r="E113" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// === Scriptlets</v>
       </c>
     </row>
@@ -4373,7 +4414,7 @@
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// --- Basic scriptlets</v>
       </c>
     </row>
@@ -4385,7 +4426,7 @@
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %postin script is executed right after the package got installed</v>
       </c>
     </row>
@@ -4401,8 +4442,8 @@
       </c>
       <c r="D116" s="1"/>
       <c r="E116" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postin = 1024, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postin = 1024, // (string) </v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -4417,8 +4458,8 @@
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postinflags = 5021, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postinflags = 5021, // (int32) </v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4433,8 +4474,8 @@
       </c>
       <c r="D118" s="1"/>
       <c r="E118" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postinprog = 1086, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postinprog = 1086, // (string array) </v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4445,7 +4486,7 @@
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %posttrans scripts are all executed at the end of the transaction that installed their packages</v>
       </c>
     </row>
@@ -4461,8 +4502,8 @@
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Posttrans = 1152, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Posttrans = 1152, // (string) </v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4477,8 +4518,8 @@
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Posttransflags = 5025, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Posttransflags = 5025, // (int32) </v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4493,8 +4534,8 @@
       </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Posttransprog = 1154, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Posttransprog = 1154, // (string array) </v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4505,7 +4546,7 @@
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %postuntrans scripts are all executed at the end of the transaction that removes their packages</v>
       </c>
     </row>
@@ -4521,8 +4562,8 @@
       </c>
       <c r="D124" s="1"/>
       <c r="E124" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postuntrans = 5104, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postuntrans = 5104, // (string) </v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4537,8 +4578,8 @@
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postuntransflags = 5108, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postuntransflags = 5108, // (int32) </v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4553,8 +4594,8 @@
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postuntransprog = 5106, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postuntransprog = 5106, // (string array) </v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4565,7 +4606,7 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %postun script is executed right after the package was removed</v>
       </c>
     </row>
@@ -4581,8 +4622,8 @@
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postun = 1026, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postun = 1026, // (string) </v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4597,8 +4638,8 @@
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postunflags = 5023, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postunflags = 5023, // (int32) </v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4613,8 +4654,8 @@
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Postunprog = 1088, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Postunprog = 1088, // (string array) </v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4625,7 +4666,7 @@
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
       <c r="E131" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %prein script is executed right before the package is installed</v>
       </c>
     </row>
@@ -4641,8 +4682,8 @@
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Prein = 1023, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Prein = 1023, // (string) </v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -4657,8 +4698,8 @@
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preinflags = 5020, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preinflags = 5020, // (int32) </v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4673,8 +4714,8 @@
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preinprog = 1085, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preinprog = 1085, // (string array) </v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="30">
@@ -4685,7 +4726,7 @@
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %pretrans scripts are executed for to be installed packages before any packages are installed/removed</v>
       </c>
     </row>
@@ -4701,8 +4742,8 @@
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Pretrans = 1151, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Pretrans = 1151, // (string) </v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -4717,8 +4758,8 @@
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Pretransflags = 5024, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Pretransflags = 5024, // (int32) </v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4733,8 +4774,8 @@
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Pretransprog = 1153, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Pretransprog = 1153, // (string array) </v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="30">
@@ -4745,7 +4786,7 @@
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %preuntrans scripts are executed for to be removed packages before any packages are installed/removed</v>
       </c>
     </row>
@@ -4761,8 +4802,8 @@
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preuntrans = 5103, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preuntrans = 5103, // (string) </v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -4777,8 +4818,8 @@
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preuntransflags = 5107, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preuntransflags = 5107, // (int32) </v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -4793,8 +4834,8 @@
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preuntransprog = 5105, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preuntransprog = 5105, // (string array) </v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -4805,7 +4846,7 @@
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %preun script is executed right before the package gets removed</v>
       </c>
     </row>
@@ -4821,8 +4862,8 @@
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preun = 1025, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preun = 1025, // (string) </v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -4837,8 +4878,8 @@
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preunflags = 5022, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preunflags = 5022, // (int32) </v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -4853,8 +4894,8 @@
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Preunprog = 1087, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Preunprog = 1087, // (string array) </v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -4865,7 +4906,7 @@
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// %verify script is executed when the package is verified (e.g. with rpm -V)</v>
       </c>
     </row>
@@ -4881,8 +4922,8 @@
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Verifyscript = 1079, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Verifyscript = 1079, // (string) </v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -4897,8 +4938,8 @@
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Verifyscriptflags = 5026, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Verifyscriptflags = 5026, // (int32) </v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -4913,8 +4954,8 @@
       </c>
       <c r="D150" s="1"/>
       <c r="E150" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Verifyscriptprog = 1091, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Verifyscriptprog = 1091, // (string array) </v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="18">
@@ -4925,7 +4966,7 @@
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// --- Triggers</v>
       </c>
     </row>
@@ -4941,8 +4982,8 @@
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggerflags = 1068, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Triggerflags = 1068, // (int32 array) </v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -4957,8 +4998,8 @@
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggerindex = 1069, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Triggerindex = 1069, // (int32 array) </v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -4973,8 +5014,8 @@
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggername = 1066, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Triggername = 1066, // (string array) </v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -4989,8 +5030,8 @@
       </c>
       <c r="D155" s="1"/>
       <c r="E155" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggerscriptflags = 5027, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Triggerscriptflags = 5027, // (int32 array) </v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5005,8 +5046,8 @@
       </c>
       <c r="D156" s="1"/>
       <c r="E156" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggerscriptprog = 1092, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Triggerscriptprog = 1092, // (string array) </v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -5021,8 +5062,8 @@
       </c>
       <c r="D157" s="1"/>
       <c r="E157" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggerscripts = 1065, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Triggerscripts = 1065, // (string array) </v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5037,8 +5078,8 @@
       </c>
       <c r="D158" s="1"/>
       <c r="E158" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggerversion = 1067, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Triggerversion = 1067, // (string array) </v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="18">
@@ -5049,7 +5090,7 @@
       </c>
       <c r="D159" s="1"/>
       <c r="E159" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// --- File triggers</v>
       </c>
     </row>
@@ -5065,8 +5106,8 @@
       </c>
       <c r="D160" s="1"/>
       <c r="E160" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerflags = 5072, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggerflags = 5072, // (int32 array) </v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -5081,8 +5122,8 @@
       </c>
       <c r="D161" s="1"/>
       <c r="E161" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerindex = 5070, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggerindex = 5070, // (int32 array) </v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -5097,8 +5138,8 @@
       </c>
       <c r="D162" s="1"/>
       <c r="E162" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggername = 5069, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggername = 5069, // (string array) </v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5113,8 +5154,8 @@
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerpriorities = 5084, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggerpriorities = 5084, // (int32 array) </v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5129,8 +5170,8 @@
       </c>
       <c r="D164" s="1"/>
       <c r="E164" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerscriptflags = 5068, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggerscriptflags = 5068, // (int32 array) </v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -5145,8 +5186,8 @@
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerscriptprog = 5067, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggerscriptprog = 5067, // (string array) </v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5161,8 +5202,8 @@
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerscripts = 5066, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggerscripts = 5066, // (string array) </v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5177,8 +5218,8 @@
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerversion = 5071, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filetriggerversion = 5071, // (string array) </v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5193,8 +5234,8 @@
       </c>
       <c r="D168" s="1"/>
       <c r="E168" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerflags = 5082, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggerflags = 5082, // (int32 array) </v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -5209,8 +5250,8 @@
       </c>
       <c r="D169" s="1"/>
       <c r="E169" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerindex = 5080, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggerindex = 5080, // (int32 array) </v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -5225,8 +5266,8 @@
       </c>
       <c r="D170" s="1"/>
       <c r="E170" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggername = 5079, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggername = 5079, // (string array) </v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5241,8 +5282,8 @@
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerpriorities = 5085, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggerpriorities = 5085, // (int32 array) </v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5257,8 +5298,8 @@
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerscriptflags = 5078, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggerscriptflags = 5078, // (int32 array) </v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5273,8 +5314,8 @@
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerscriptprog = 5077, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggerscriptprog = 5077, // (string array) </v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5289,8 +5330,8 @@
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerscripts = 5076, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggerscripts = 5076, // (string array) </v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5305,390 +5346,374 @@
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerversion = 5081, // string array</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" ht="24">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Transfiletriggerversion = 5081, // (string array) </v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
-      <c r="D176" s="3" t="s">
+      <c r="D176" s="1"/>
+      <c r="E176" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">// === </v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="24">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1"/>
+      <c r="D177" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="E176" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
+      <c r="E177" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
         <v>// === Signatures and digests</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5">
-      <c r="A177" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B177" s="1">
-        <v>267</v>
-      </c>
-      <c r="C177" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D177" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E177" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Dsaheader = 267, // bin</v>
       </c>
     </row>
     <row r="178" spans="1:5">
       <c r="A178" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B178" s="1">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E178" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Longsigsize = 270, // int64</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Dsaheader = 267, // (bin) OpenPGP DSA signature of the header (if thus signed)</v>
       </c>
     </row>
     <row r="179" spans="1:5">
       <c r="A179" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B179" s="1">
-        <v>5092</v>
+        <v>270</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E179" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Payloaddigest = 5092, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Longsigsize = 270, // (int64) Header+payload size if &gt; 4GB.</v>
       </c>
     </row>
     <row r="180" spans="1:5">
       <c r="A180" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B180" s="1">
-        <v>5093</v>
+        <v>5092</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E180" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Payloaddigestalgo = 5093, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Payloaddigest = 5092, // (string array) Cryptographic digest of the compressed payload.</v>
       </c>
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B181" s="1">
-        <v>5097</v>
+        <v>5093</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E181" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Payloaddigestalt = 5097, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Payloaddigestalgo = 5093, // (int32) ID of the payload digest algorithm.</v>
       </c>
     </row>
     <row r="182" spans="1:5">
       <c r="A182" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B182" s="1">
-        <v>268</v>
+        <v>5097</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E182" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Rsaheader = 268, // bin</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Payloaddigestalt = 5097, // (string array) Cryptographic digest of the uncompressed payload.</v>
       </c>
     </row>
     <row r="183" spans="1:5">
       <c r="A183" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B183" s="1">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E183" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sha1header = 269, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Rsaheader = 268, // (bin) OpenPGP RSA signature of the header (if thus signed).</v>
       </c>
     </row>
     <row r="184" spans="1:5">
       <c r="A184" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B184" s="1">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E184" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sha256header = 273, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sha1header = 269, // (string) SHA1 digest of the header.</v>
       </c>
     </row>
     <row r="185" spans="1:5">
       <c r="A185" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B185" s="1">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E185" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Siggpg = 262, // bin</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sha256header = 273, // (string) SHA256 digest of the header.</v>
       </c>
     </row>
     <row r="186" spans="1:5">
       <c r="A186" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B186" s="1">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E186" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sigmd5 = 261, // bin</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Siggpg = 262, // (bin) OpenPGP DSA signature of the header+payload (if thus signed).</v>
       </c>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B187" s="1">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>67</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E187" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sigpgp = 259, // bin</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sigmd5 = 261, // (bin) MD5 digest of the header+payload.</v>
       </c>
     </row>
     <row r="188" spans="1:5">
       <c r="A188" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B188" s="1">
+        <v>259</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E188" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sigpgp = 259, // (bin) OpenPGP RSA signature of the header+payload (if thus signed).</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B188" s="1">
+      <c r="B189" s="1">
         <v>257</v>
       </c>
-      <c r="C188" s="1" t="s">
+      <c r="C189" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D188" s="1" t="s">
+      <c r="D189" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E188" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sigsize = 257, // int32</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" ht="24">
-      <c r="A189" s="1"/>
-      <c r="B189" s="1"/>
-      <c r="C189" s="1"/>
-      <c r="D189" s="3" t="s">
-        <v>278</v>
-      </c>
       <c r="E189" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>// === Installed package headers only</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sigsize = 257, // (int32) Header+payload size.</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" ht="15" customHeight="1">
       <c r="A190" s="1" t="s">
-        <v>279</v>
+        <v>409</v>
       </c>
       <c r="B190" s="1">
-        <v>1029</v>
+        <v>62</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D190" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E190" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filestates = 1029, // char array</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5">
+        <v>410</v>
+      </c>
+      <c r="D190" s="3"/>
+      <c r="E190" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">HEADERSIGNATURES = 62, // (BIN) </v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" ht="15" customHeight="1">
       <c r="A191" s="1" t="s">
-        <v>282</v>
+        <v>411</v>
       </c>
       <c r="B191" s="1">
-        <v>1127</v>
+        <v>267</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="E191" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Installcolor = 1127, // int32</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5">
+        <v>410</v>
+      </c>
+      <c r="D191" s="3"/>
+      <c r="E191" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">DSA = 267, // (BIN) </v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" ht="15" customHeight="1">
       <c r="A192" s="1" t="s">
-        <v>284</v>
+        <v>412</v>
       </c>
       <c r="B192" s="1">
-        <v>1128</v>
+        <v>268</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D192" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="E192" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Installtid = 1128, // int32</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5">
+        <v>410</v>
+      </c>
+      <c r="D192" s="3"/>
+      <c r="E192" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">RSA = 268, // (BIN) </v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" ht="15" customHeight="1">
       <c r="A193" s="1" t="s">
-        <v>286</v>
+        <v>413</v>
       </c>
       <c r="B193" s="1">
-        <v>1008</v>
+        <v>272</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E193" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Installtime = 1008, // int32</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5">
+        <v>414</v>
+      </c>
+      <c r="D193" s="3"/>
+      <c r="E193" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">SHA256 = 272, // (STRING) </v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" ht="15" customHeight="1">
       <c r="A194" s="1" t="s">
-        <v>288</v>
+        <v>415</v>
       </c>
       <c r="B194" s="1">
-        <v>1099</v>
+        <v>274</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D194" s="1"/>
-      <c r="E194" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Instprefixes = 1099, // string array</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5">
+        <v>416</v>
+      </c>
+      <c r="D194" s="3"/>
+      <c r="E194" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">FILESIGNATURES = 274, // (STRING_ARRAY) </v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" ht="15" customHeight="1">
       <c r="A195" s="1" t="s">
-        <v>289</v>
+        <v>417</v>
       </c>
       <c r="B195" s="1">
-        <v>1120</v>
+        <v>276</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D195" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E195" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Origbasenames = 1120, // string array</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5">
+        <v>416</v>
+      </c>
+      <c r="D195" s="3"/>
+      <c r="E195" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">VERITYSIGNATURES = 276, // (STRING_ARRAY) </v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" ht="15" customHeight="1">
       <c r="A196" s="1" t="s">
-        <v>291</v>
+        <v>418</v>
       </c>
       <c r="B196" s="1">
-        <v>1119</v>
+        <v>277</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D196" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E196" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Origdirindexes = 1119, // int32 array</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5">
+        <v>419</v>
+      </c>
+      <c r="D196" s="3"/>
+      <c r="E196" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">VERITYSIGNATUREALGO = 277, // (INT_32) </v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" ht="15" customHeight="1">
       <c r="A197" s="1" t="s">
-        <v>293</v>
+        <v>420</v>
       </c>
       <c r="B197" s="1">
-        <v>1121</v>
+        <v>999</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E197" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Origdirnames = 1121, // string array</v>
+        <v>410</v>
+      </c>
+      <c r="D197" s="3"/>
+      <c r="E197" s="10" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">RESERVED = 999, // (BIN) </v>
       </c>
     </row>
     <row r="198" spans="1:5" ht="24">
@@ -5696,1147 +5721,1301 @@
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="3" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="E198" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>// === Source packages</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>// === Installed package headers only</v>
       </c>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="1" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="B199" s="1">
-        <v>1089</v>
+        <v>1029</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>33</v>
+        <v>280</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="E199" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Buildarchs = 1089, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filestates = 1029, // (char array) Per-file installed status information (installed/skipped/forced etc)</v>
       </c>
     </row>
     <row r="200" spans="1:5">
       <c r="A200" s="1" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="B200" s="1">
-        <v>1059</v>
+        <v>1127</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="E200" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Excludearch = 1059, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Installcolor = 1127, // (int32) “Color” of transaction in which the package was installed.</v>
       </c>
     </row>
     <row r="201" spans="1:5">
       <c r="A201" s="1" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="B201" s="1">
-        <v>1060</v>
+        <v>1128</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="E201" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Excludeos = 1060, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Installtid = 1128, // (int32) ID of transaction in which the package was installed.</v>
       </c>
     </row>
     <row r="202" spans="1:5">
       <c r="A202" s="1" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="B202" s="1">
-        <v>1061</v>
+        <v>1008</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="E202" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Exclusivearch = 1061, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Installtime = 1008, // (int32) Unix timestamp of package installation.</v>
       </c>
     </row>
     <row r="203" spans="1:5">
       <c r="A203" s="1" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="B203" s="1">
-        <v>1062</v>
+        <v>1099</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D203" s="1" t="s">
-        <v>305</v>
-      </c>
+      <c r="D203" s="1"/>
       <c r="E203" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Exclusiveos = 1062, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Instprefixes = 1099, // (string array) </v>
       </c>
     </row>
     <row r="204" spans="1:5">
       <c r="A204" s="1" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="B204" s="1">
-        <v>1052</v>
+        <v>1120</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="E204" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Nopatch = 1052, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Origbasenames = 1120, // (string array) Original Basenames (relocated packages only)</v>
       </c>
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="1" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="B205" s="1">
-        <v>1051</v>
+        <v>1119</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="E205" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Nosource = 1051, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Origdirindexes = 1119, // (int32 array) Original Dirindexes (relocated packages only)</v>
       </c>
     </row>
     <row r="206" spans="1:5">
       <c r="A206" s="1" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="B206" s="1">
-        <v>1019</v>
+        <v>1121</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="E206" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Patch = 1019, // string array</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5">
-      <c r="A207" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="B207" s="1">
-        <v>1018</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D207" s="1" t="s">
-        <v>313</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Origdirnames = 1121, // (string array) Original Dirnames (relocated packages only)</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" ht="24">
+      <c r="A207" s="1"/>
+      <c r="B207" s="1"/>
+      <c r="C207" s="1"/>
+      <c r="D207" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="E207" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Source = 1018, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>// === Source packages</v>
       </c>
     </row>
     <row r="208" spans="1:5">
       <c r="A208" s="1" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="B208" s="1">
-        <v>1106</v>
+        <v>1089</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="E208" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sourcepackage = 1106, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Buildarchs = 1089, // (string array) If present, specifies the architectures the package may be built for.</v>
       </c>
     </row>
     <row r="209" spans="1:5">
       <c r="A209" s="1" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="B209" s="1">
-        <v>5099</v>
+        <v>1059</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="E209" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Spec = 5099, // string</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" ht="24">
-      <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
-      <c r="C210" s="1"/>
-      <c r="D210" s="3" t="s">
-        <v>318</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Excludearch = 1059, // (string array) If present, limits the architectures on which the package is buildable by excluding those specified.</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B210" s="1">
+        <v>1060</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>301</v>
       </c>
       <c r="E210" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>// === Internal / special</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Excludeos = 1060, // (string array) If present, limits the operating systems on which the package is buildable by excluding those specified.</v>
       </c>
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="1" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="B211" s="1">
-        <v>100</v>
+        <v>1061</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="E211" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Headeri18ntable = 100, // string array</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" ht="30">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Exclusivearch = 1061, // (string array) If present, limits the architectures on which the package is buildable exclusively to those specified.</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
       <c r="A212" s="1" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="B212" s="1">
-        <v>63</v>
+        <v>1062</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="E212" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Headerimmutable = 63, // bin</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Exclusiveos = 1062, // (string array) If present, limits the operating systems on which the package is buildable exclusively to those specified.</v>
       </c>
     </row>
     <row r="213" spans="1:5">
       <c r="A213" s="1" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="B213" s="1">
-        <v>266</v>
+        <v>1052</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="E213" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Pubkeys = 266, // string array</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" ht="24">
-      <c r="A214" s="1"/>
-      <c r="B214" s="1"/>
-      <c r="C214" s="1"/>
-      <c r="D214" s="3" t="s">
-        <v>325</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Nopatch = 1052, // (int32 array) Denotes a patch number for which source is not supplied.</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B214" s="1">
+        <v>1051</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="E214" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>// === Deprecated / Obsolete</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Nosource = 1051, // (int32 array) Denotes a source number for which source is not supplied.</v>
       </c>
     </row>
     <row r="215" spans="1:5">
       <c r="A215" s="1" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="B215" s="1">
-        <v>1147</v>
+        <v>1019</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D215" s="1"/>
+      <c r="D215" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="E215" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filecontexts = 1147, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Patch = 1019, // (string array) Patch file names.</v>
       </c>
     </row>
     <row r="216" spans="1:5">
       <c r="A216" s="1" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="B216" s="1">
-        <v>1148</v>
+        <v>1018</v>
       </c>
       <c r="C216" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D216" s="1"/>
+      <c r="D216" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="E216" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fscontexts = 1148, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Source = 1018, // (string array) Source file names.</v>
       </c>
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="1" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="B217" s="1">
-        <v>1012</v>
+        <v>1106</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D217" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="E217" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Gif = 1012, // bin</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sourcepackage = 1106, // (int32) Denotes a source rpm.</v>
       </c>
     </row>
     <row r="218" spans="1:5">
       <c r="A218" s="1" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="B218" s="1">
-        <v>1043</v>
+        <v>5099</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D218" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="E218" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Icon = 1043, // bin</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5">
-      <c r="A219" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="B219" s="1">
-        <v>1159</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D219" s="1"/>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Spec = 5099, // (string) Expanded and parsed spec contents.</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" ht="24">
+      <c r="A219" s="1"/>
+      <c r="B219" s="1"/>
+      <c r="C219" s="1"/>
+      <c r="D219" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="E219" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Oldenhancesname = 1159, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>// === Internal / special</v>
       </c>
     </row>
     <row r="220" spans="1:5">
       <c r="A220" s="1" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="B220" s="1">
-        <v>1160</v>
+        <v>100</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D220" s="1"/>
+      <c r="D220" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="E220" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Oldenhancesversion = 1160, // string array</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Headeri18ntable = 100, // (string array) Locales for which the header has translations.</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" ht="30">
       <c r="A221" s="1" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="B221" s="1">
-        <v>1161</v>
+        <v>63</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D221" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="E221" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Oldenhancesflags = 1161, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Headerimmutable = 63, // (bin) Special tag to return the unmodified, original image of the header even after data has been added to it in eg installation.</v>
       </c>
     </row>
     <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="B222" s="1">
-        <v>1027</v>
+        <v>266</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D222" s="1"/>
+      <c r="D222" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="E222" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Oldfilenames = 1027, // string array</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5">
-      <c r="A223" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="B223" s="1">
-        <v>1156</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D223" s="1"/>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Pubkeys = 266, // (string array) used in gpg-pubkey special packages in the RPM data base</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="24">
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
+      <c r="D223" s="3" t="s">
+        <v>325</v>
+      </c>
       <c r="E223" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Oldsuggestsname = 1156, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>// === Deprecated / Obsolete</v>
       </c>
     </row>
     <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="B224" s="1">
-        <v>1157</v>
+        <v>1147</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Oldsuggestsversion = 1157, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Filecontexts = 1147, // (string array) </v>
       </c>
     </row>
     <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="B225" s="1">
-        <v>1158</v>
+        <v>1148</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D225" s="1"/>
       <c r="E225" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Oldsuggestsflags = 1158, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Fscontexts = 1148, // (string array) </v>
       </c>
     </row>
     <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="B226" s="1">
-        <v>1134</v>
+        <v>1012</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D226" s="1"/>
       <c r="E226" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Patchesflags = 1134, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Gif = 1012, // (bin) </v>
       </c>
     </row>
     <row r="227" spans="1:5">
       <c r="A227" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B227" s="1">
-        <v>1133</v>
+        <v>1043</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="D227" s="1"/>
       <c r="E227" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Patchesname = 1133, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Icon = 1043, // (bin) </v>
       </c>
     </row>
     <row r="228" spans="1:5">
       <c r="A228" s="1" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B228" s="1">
-        <v>1135</v>
+        <v>1159</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D228" s="1"/>
       <c r="E228" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Patchesversion = 1135, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Oldenhancesname = 1159, // (string array) </v>
       </c>
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="B229" s="1">
-        <v>1149</v>
+        <v>1160</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D229" s="1"/>
       <c r="E229" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Recontexts = 1149, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Oldenhancesversion = 1160, // (string array) </v>
       </c>
     </row>
     <row r="230" spans="1:5">
       <c r="A230" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="B230" s="1">
-        <v>1129</v>
+        <v>1161</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D230" s="1"/>
       <c r="E230" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Removetid = 1129, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Oldenhancesflags = 1161, // (int32 array) </v>
       </c>
     </row>
     <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B231" s="1">
-        <v>1013</v>
+        <v>1027</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D231" s="1"/>
       <c r="E231" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Xpm = 1013, // bin</v>
-      </c>
-    </row>
-    <row r="232" spans="1:5" ht="24">
-      <c r="A232" s="1"/>
-      <c r="B232" s="1"/>
-      <c r="C232" s="1"/>
-      <c r="D232" s="3" t="s">
-        <v>343</v>
-      </c>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Oldfilenames = 1027, // (string array) </v>
+      </c>
+    </row>
+    <row r="232" spans="1:5">
+      <c r="A232" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B232" s="1">
+        <v>1156</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D232" s="1"/>
       <c r="E232" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>// === Extensions</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Oldsuggestsname = 1156, // (string array) </v>
       </c>
     </row>
     <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B233" s="1">
-        <v>5098</v>
+        <v>1157</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D233" s="1" t="s">
-        <v>345</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D233" s="1"/>
       <c r="E233" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Archsuffix = 5098, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Oldsuggestsversion = 1157, // (string array) </v>
       </c>
     </row>
     <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B234" s="1">
-        <v>1195</v>
+        <v>1158</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D234" s="1" t="s">
-        <v>347</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D234" s="1"/>
       <c r="E234" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Dbinstance = 1195, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Oldsuggestsflags = 1158, // (int32 array) </v>
       </c>
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="B235" s="1">
-        <v>5019</v>
+        <v>1134</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>349</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D235" s="1"/>
       <c r="E235" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Epochnum = 5019, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Patchesflags = 1134, // (int32 array) </v>
       </c>
     </row>
     <row r="236" spans="1:5">
       <c r="A236" s="1" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="B236" s="1">
-        <v>5013</v>
+        <v>1133</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>351</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D236" s="1"/>
       <c r="E236" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Evr = 5013, // string</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" ht="30">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Patchesname = 1133, // (string array) </v>
+      </c>
+    </row>
+    <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
-        <v>408</v>
+        <v>339</v>
       </c>
       <c r="B237" s="1">
-        <v>1141</v>
+        <v>1135</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D237" s="1" t="s">
-        <v>352</v>
-      </c>
+      <c r="D237" s="1"/>
       <c r="E237" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fileclass2 = 1141, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Patchesversion = 1135, // (string array) </v>
       </c>
     </row>
     <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="B238" s="1">
-        <v>5017</v>
+        <v>1149</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D238" s="1" t="s">
-        <v>354</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D238" s="1"/>
       <c r="E238" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Headercolor = 5017, // int32</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Recontexts = 1149, // (string array) </v>
       </c>
     </row>
     <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="B239" s="1">
-        <v>5015</v>
+        <v>1129</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D239" s="1" t="s">
-        <v>356</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D239" s="1"/>
       <c r="E239" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Nevr = 5015, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Removetid = 1129, // (int32) </v>
       </c>
     </row>
     <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="B240" s="1">
-        <v>5016</v>
+        <v>1013</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>358</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="D240" s="1"/>
       <c r="E240" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Nevra = 5016, // string</v>
-      </c>
-    </row>
-    <row r="241" spans="1:5">
-      <c r="A241" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="B241" s="1">
-        <v>5014</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D241" s="1" t="s">
-        <v>360</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v xml:space="preserve">Xpm = 1013, // (bin) </v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" ht="24">
+      <c r="A241" s="1"/>
+      <c r="B241" s="1"/>
+      <c r="C241" s="1"/>
+      <c r="D241" s="3" t="s">
+        <v>343</v>
       </c>
       <c r="E241" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Nvr = 5014, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>// === Extensions</v>
       </c>
     </row>
     <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="B242" s="1">
-        <v>1196</v>
+        <v>5098</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
       <c r="E242" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Nvra = 1196, // string</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Archsuffix = 5098, // (string) Package file arch suffix (“.src”, “.nosrc” or .arch)</v>
       </c>
     </row>
     <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="B243" s="1">
-        <v>5000</v>
+        <v>1195</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>364</v>
+        <v>347</v>
       </c>
       <c r="E243" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filenames = 5000, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Dbinstance = 1195, // (int32) Header ID of installed package, 0 otherwise.</v>
       </c>
     </row>
     <row r="244" spans="1:5">
       <c r="A244" s="1" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
       <c r="B244" s="1">
-        <v>5045</v>
+        <v>5019</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>366</v>
+        <v>349</v>
       </c>
       <c r="E244" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filenlinks = 5045, // int32 array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Epochnum = 5019, // (int32) Package epoch as numeric value (0 if not present).</v>
       </c>
     </row>
     <row r="245" spans="1:5">
       <c r="A245" s="1" t="s">
-        <v>367</v>
+        <v>350</v>
       </c>
       <c r="B245" s="1">
-        <v>5001</v>
+        <v>5013</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="E245" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Fileprovide = 5001, // string array</v>
-      </c>
-    </row>
-    <row r="246" spans="1:5">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Evr = 5013, // (string) Formatted epoch:version-release string of the package</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" ht="45">
       <c r="A246" s="1" t="s">
-        <v>369</v>
+        <v>421</v>
       </c>
       <c r="B246" s="1">
-        <v>5002</v>
+        <v>1141</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="E246" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filerequire = 5002, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>FileClass = 1141, // (string array) Per-file formatted libmagic classification strings, calculated from the Fileclass and Classdict tags. Note overlap with the concrete Fileclass tag with different type (integer array)!</v>
       </c>
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="1" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="B247" s="1">
-        <v>5040</v>
+        <v>5017</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="E247" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Instfilenames = 5040, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Headercolor = 5017, // (int32) Header “color” calculated from file colors.</v>
       </c>
     </row>
     <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="B248" s="1">
-        <v>5007</v>
+        <v>5015</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="E248" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Origfilenames = 5007, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Nevr = 5015, // (string) Formatted name-epoch:version-release string of the package</v>
       </c>
     </row>
     <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="B249" s="1">
-        <v>5042</v>
+        <v>5016</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="E249" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Providenevrs = 5042, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Nevra = 5016, // (string) Formatted name-epoch:version-release.arch string of the package</v>
       </c>
     </row>
     <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="B250" s="1">
-        <v>5044</v>
+        <v>5014</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="E250" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Conflictnevrs = 5044, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Nvr = 5014, // (string) Formatted name-version-release string of the package</v>
       </c>
     </row>
     <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="B251" s="1">
-        <v>5043</v>
+        <v>1196</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="E251" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Obsoletenevrs = 5043, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Nvra = 1196, // (string) Formatted name-version-release.arch string of the package</v>
       </c>
     </row>
     <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="B252" s="1">
-        <v>5061</v>
+        <v>5000</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="E252" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Enhancenevrs = 5061, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filenames = 5000, // (string array) Per file paths contained in the package, calculated from the path triplet.</v>
       </c>
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="B253" s="1">
-        <v>5058</v>
+        <v>5045</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="E253" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Recommendnevrs = 5058, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filenlinks = 5045, // (int32 array) Per file hardlink number, calculated from inode/device information.</v>
       </c>
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="B254" s="1">
-        <v>5041</v>
+        <v>5001</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
       <c r="E254" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Requirenevrs = 5041, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Fileprovide = 5001, // (string array) Per file dependency capabilities provided by the corresponding files.</v>
       </c>
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="B255" s="1">
-        <v>5059</v>
+        <v>5002</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="E255" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Suggestnevrs = 5059, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filerequire = 5002, // (string array) Per file dependency capabilities required by the corresponding files.</v>
       </c>
     </row>
     <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="B256" s="1">
-        <v>5060</v>
+        <v>5040</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="E256" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Supplementnevrs = 5060, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Instfilenames = 5040, // (string array) Per file paths installed from the package, calculated from the path triplet and file status info.</v>
       </c>
     </row>
     <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="B257" s="1">
-        <v>5109</v>
+        <v>5007</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="E257" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Sysusers = 5109, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Origfilenames = 5007, // (string array) Original Filenames in relocated packages.</v>
       </c>
     </row>
     <row r="258" spans="1:5">
       <c r="A258" s="1" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="B258" s="1">
-        <v>5086</v>
+        <v>5042</v>
       </c>
       <c r="C258" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="E258" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggerconds = 5086, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Providenevrs = 5042, // (string array) Formatted name [op version] provide dependency strings.</v>
       </c>
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="1" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="B259" s="1">
-        <v>5087</v>
+        <v>5044</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="E259" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Filetriggertype = 5087, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Conflictnevrs = 5044, // (string array) Formatted name [op version] conflict dependency strings.</v>
       </c>
     </row>
     <row r="260" spans="1:5">
       <c r="A260" s="1" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="B260" s="1">
-        <v>5088</v>
+        <v>5043</v>
       </c>
       <c r="C260" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="E260" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggerconds = 5088, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Obsoletenevrs = 5043, // (string array) Formatted name [op version] obsolete dependency strings.</v>
       </c>
     </row>
     <row r="261" spans="1:5">
       <c r="A261" s="1" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="B261" s="1">
-        <v>5089</v>
+        <v>5061</v>
       </c>
       <c r="C261" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="E261" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Transfiletriggertype = 5089, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Enhancenevrs = 5061, // (string array) Formatted name [op version] enhance dependency strings.</v>
       </c>
     </row>
     <row r="262" spans="1:5">
       <c r="A262" s="1" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="B262" s="1">
-        <v>5005</v>
+        <v>5058</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="E262" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggerconds = 5005, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Recommendnevrs = 5058, // (string array) Formatted name [op version] recommend dependency strings.</v>
       </c>
     </row>
     <row r="263" spans="1:5">
       <c r="A263" s="1" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="B263" s="1">
-        <v>5006</v>
+        <v>5041</v>
       </c>
       <c r="C263" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="E263" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Triggertype = 5006, // string array</v>
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Requirenevrs = 5041, // (string array) Formatted name [op version] require dependency strings.</v>
       </c>
     </row>
     <row r="264" spans="1:5">
       <c r="A264" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B264" s="1">
+        <v>5059</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="E264" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Suggestnevrs = 5059, // (string array) Formatted name [op version] suggest dependency strings.</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5">
+      <c r="A265" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B265" s="1">
+        <v>5060</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E265" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Supplementnevrs = 5060, // (string array) Formatted name [op version] supplement dependency strings.</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5">
+      <c r="A266" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B266" s="1">
+        <v>5109</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E266" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Sysusers = 5109, // (string array) Formatted systemd-sysusers lines for the package.</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5">
+      <c r="A267" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B267" s="1">
+        <v>5086</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E267" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filetriggerconds = 5086, // (string array) Formatted file trigger condition information.</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
+      <c r="A268" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B268" s="1">
+        <v>5087</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E268" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Filetriggertype = 5087, // (string array) Formatted file trigger type information.</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5">
+      <c r="A269" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B269" s="1">
+        <v>5088</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E269" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Transfiletriggerconds = 5088, // (string array) Formatted transaction file trigger condition information.</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5">
+      <c r="A270" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B270" s="1">
+        <v>5089</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E270" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Transfiletriggertype = 5089, // (string array) Formatted transaction file trigger type information.</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5">
+      <c r="A271" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B271" s="1">
+        <v>5005</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E271" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Triggerconds = 5005, // (string array) Formatted trigger condition information.</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B272" s="1">
+        <v>5006</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E272" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Triggertype = 5006, // (string array) Formatted trigger type information.</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="B264" s="1">
+      <c r="B273" s="1">
         <v>5018</v>
       </c>
-      <c r="C264" s="1" t="s">
+      <c r="C273" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D264" s="1" t="s">
+      <c r="D273" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="E264" s="1" t="str">
-        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // "&amp;Tableau1[[#This Row],[Type]]))</f>
-        <v>Verbose = 5018, // int32</v>
+      <c r="E273" s="1" t="str">
+        <f>IF(ISBLANK(Tableau1[[#This Row],[Tag]]),IF(ISBLANK(Tableau1[[#This Row],[Type]]),"// === "&amp;Tableau1[[#This Row],[Description]],"// --- "&amp;Tableau1[[#This Row],[Type]]),IF(ISBLANK(Tableau1[[#This Row],[Value]]),"// "&amp;Tableau1[[#This Row],[Tag]],Tableau1[[#This Row],[Tag]]&amp;" = "&amp;Tableau1[[#This Row],[Value]]&amp;", // ("&amp;Tableau1[[#This Row],[Type]]&amp;") "&amp;Tableau1[[#This Row],[Description]]))</f>
+        <v>Verbose = 5018, // (int32) Returns 1 if rpm is running in verbose mode.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>